<commit_message>
new data files and responding to assorted researcher edits
</commit_message>
<xml_diff>
--- a/data/AssetSubsidies.xlsx
+++ b/data/AssetSubsidies.xlsx
@@ -1,16 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\LHP\SMcKerna\Nine Charts 2017\Files for Ben\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="17235" windowHeight="8760"/>
+    <workbookView xWindow="240" yWindow="1020" windowWidth="17235" windowHeight="8760" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Asset Subsidies" sheetId="1" r:id="rId1"/>
+    <sheet name="Asset Subsidies--%s and dollars" sheetId="2" r:id="rId1"/>
+    <sheet name="Asset Subsidies--dollars" sheetId="1" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
     <definedName name="A">[1]CI!$A$7:$BL$313</definedName>
@@ -18,15 +24,12 @@
     <definedName name="B">#REF!</definedName>
     <definedName name="C_">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
-  <si>
-    <t>Percentage share by taxpayer income quintile</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
   <si>
     <t>Expenditure</t>
   </si>
@@ -70,53 +73,6 @@
     <t>Saver's credit</t>
   </si>
   <si>
-    <t>Size and Distribution of Select Asset-Building Tax Subsidies, 2013</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Source: </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Steuerle et al. (2014)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Note: “Income” refers to the Tax Policy Center’s “expanded cash income” measure, which is described in </t>
-    </r>
-    <r>
-      <rPr>
-        <u/>
-        <sz val="11"/>
-        <color theme="10"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Rosenberg (2013).</t>
-    </r>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -138,16 +94,101 @@
       <t>http://urbn.is/wealthcharts</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Updated estimates from </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Steuerle et al. (2014)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: “Income” refers to the Tax Policy Center’s “expanded cash income” measure, which is described in </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Rosenberg (2013).</t>
+    </r>
+  </si>
+  <si>
+    <t>Size and Distribution of Select Asset-Building Tax Subsidies, 2017</t>
+  </si>
+  <si>
+    <t>FINAL CHART VALUES</t>
+  </si>
+  <si>
+    <t>Dollars by taxpayer income quintile (billions)</t>
+  </si>
+  <si>
+    <t>Total Expenditure and Share of Benefit, 2017</t>
+  </si>
+  <si>
+    <t>Comms: Use this sheet for downloadable data</t>
+  </si>
+  <si>
+    <t>Comms: Use this sheet for the data that will feed the graphic</t>
+  </si>
+  <si>
+    <t>Share by taxpayer income quintile</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0_);[Red]\(&quot;$&quot;#,##0.0\)"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +232,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -202,8 +258,14 @@
     <fill>
       <patternFill patternType="lightUp"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -220,6 +282,15 @@
       </right>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -239,12 +310,18 @@
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="13" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -267,6 +344,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -23733,7 +23813,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -23766,9 +23846,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -23801,6 +23898,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -23977,189 +24091,417 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:I16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A25" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="37" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" s="8"/>
+    </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.1</v>
+      </c>
+      <c r="C5">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="D5">
+        <v>6.7</v>
+      </c>
+      <c r="E5">
+        <v>19.5</v>
+      </c>
+      <c r="F5">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="G5" s="4">
+        <v>63.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>0.1</v>
+      </c>
+      <c r="C6">
+        <v>1.2</v>
+      </c>
+      <c r="D6">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="E6">
+        <v>23.7</v>
+      </c>
+      <c r="F6">
+        <v>66.599999999999994</v>
+      </c>
+      <c r="G6" s="4">
+        <v>33.299999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9">
+      <c r="A7" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>0.5</v>
+      </c>
+      <c r="C8">
+        <v>3.7</v>
+      </c>
+      <c r="D8">
+        <v>10.6</v>
+      </c>
+      <c r="E8">
+        <v>22.5</v>
+      </c>
+      <c r="F8">
+        <v>62.8</v>
+      </c>
+      <c r="G8" s="4">
+        <v>194.447</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>0.7</v>
+      </c>
+      <c r="C9">
+        <v>3.9</v>
+      </c>
+      <c r="D9">
+        <v>12.2</v>
+      </c>
+      <c r="E9">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="F9">
+        <v>63</v>
+      </c>
+      <c r="G9" s="4">
+        <v>7.9720000000000013</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10">
+        <v>13.4</v>
+      </c>
+      <c r="C10">
+        <v>40.4</v>
+      </c>
+      <c r="D10">
+        <v>31.1</v>
+      </c>
+      <c r="E10">
+        <v>14.3</v>
+      </c>
+      <c r="F10">
+        <v>0.8</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2.109</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9">
+      <c r="A12" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="6"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A12" r:id="rId1" display="http://www.urban.org/publications/413241.html"/>
+    <hyperlink ref="A13" r:id="rId2" display="http://www.taxpolicycenter.org/UploadedPDF/412871-measuring-income.pdf"/>
+    <hyperlink ref="A14" r:id="rId3" display="http://urbn.is/wealthcharts"/>
+  </hyperlinks>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId4"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="34.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E3" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="4">
+        <v>6.3600000000000004E-2</v>
+      </c>
+      <c r="C5" s="4">
+        <v>0.69960000000000011</v>
+      </c>
+      <c r="D5" s="4">
+        <v>4.2612000000000005</v>
+      </c>
+      <c r="E5" s="4">
+        <v>12.402000000000001</v>
+      </c>
+      <c r="F5" s="4">
+        <v>46.1736</v>
+      </c>
+      <c r="G5" s="4">
+        <v>63.6</v>
+      </c>
+      <c r="H5" s="4"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="4">
+        <v>3.3299999999999996E-2</v>
+      </c>
+      <c r="C6" s="4">
+        <v>0.39959999999999996</v>
+      </c>
+      <c r="D6" s="4">
+        <v>2.7639</v>
+      </c>
+      <c r="E6" s="4">
+        <v>7.8920999999999992</v>
+      </c>
+      <c r="F6" s="4">
+        <v>22.177799999999994</v>
+      </c>
+      <c r="G6" s="4">
+        <v>33.266699999999993</v>
+      </c>
+      <c r="H6" s="4"/>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="4">
+        <v>0.97223500000000007</v>
+      </c>
+      <c r="C8" s="4">
+        <v>7.1945390000000007</v>
+      </c>
+      <c r="D8" s="4">
+        <v>20.611381999999999</v>
+      </c>
+      <c r="E8" s="4">
+        <v>43.750575000000005</v>
+      </c>
+      <c r="F8" s="4">
+        <v>122.11271600000001</v>
+      </c>
+      <c r="G8" s="4">
+        <v>194.64144700000003</v>
+      </c>
+      <c r="H8" s="4"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9" s="4">
+        <v>5.5804000000000006E-2</v>
+      </c>
+      <c r="C9" s="4">
+        <v>0.31090800000000007</v>
+      </c>
+      <c r="D9" s="4">
+        <v>0.97258400000000012</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1.6023720000000004</v>
+      </c>
+      <c r="F9" s="4">
+        <v>5.0223600000000008</v>
+      </c>
+      <c r="G9" s="4">
+        <v>7.9640280000000017</v>
+      </c>
+      <c r="H9" s="4"/>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="4">
+        <v>0.28260600000000002</v>
+      </c>
+      <c r="C10" s="4">
+        <v>0.8520359999999999</v>
+      </c>
+      <c r="D10" s="4">
+        <v>0.65589900000000001</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.30158700000000005</v>
+      </c>
+      <c r="F10" s="4">
+        <v>1.6872000000000002E-2</v>
+      </c>
+      <c r="G10" s="4">
+        <v>2.109</v>
+      </c>
+      <c r="H10" s="4"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="B2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="B3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-      <c r="F3" t="s">
-        <v>6</v>
-      </c>
-      <c r="G3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5">
-        <v>0.1</v>
-      </c>
-      <c r="C5">
-        <v>1.4</v>
-      </c>
-      <c r="D5">
-        <v>7.6</v>
-      </c>
-      <c r="E5">
-        <v>19.2</v>
-      </c>
-      <c r="F5">
-        <v>71.7</v>
-      </c>
-      <c r="G5" s="1">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6">
-        <v>0.1</v>
-      </c>
-      <c r="C6">
-        <v>1.6</v>
-      </c>
-      <c r="D6">
-        <v>7.9</v>
-      </c>
-      <c r="E6">
-        <v>20.7</v>
-      </c>
-      <c r="F6">
-        <v>69.7</v>
-      </c>
-      <c r="G6" s="1">
-        <v>29.3</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="A7" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="A8" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8">
-        <v>0.7</v>
-      </c>
-      <c r="C8">
-        <v>3.8</v>
-      </c>
-      <c r="D8">
-        <v>9</v>
-      </c>
-      <c r="E8">
-        <v>18</v>
-      </c>
-      <c r="F8">
-        <v>68.400000000000006</v>
-      </c>
-      <c r="G8" s="1">
-        <v>91.7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9">
-        <v>0.8</v>
-      </c>
-      <c r="C9">
-        <v>4.8</v>
-      </c>
-      <c r="D9">
-        <v>11.7</v>
-      </c>
-      <c r="E9">
-        <v>18.8</v>
-      </c>
-      <c r="F9">
-        <v>63.9</v>
-      </c>
-      <c r="G9" s="1">
-        <v>5.2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10">
-        <v>12.5</v>
-      </c>
-      <c r="C10">
-        <v>37.5</v>
-      </c>
-      <c r="D10">
-        <v>40.700000000000003</v>
-      </c>
-      <c r="E10">
-        <v>8.9</v>
-      </c>
-      <c r="F10">
-        <v>0.3</v>
-      </c>
-      <c r="G10" s="1">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="2" t="s">
+    <row r="13" spans="1:8">
+      <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
+    <row r="14" spans="1:8">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
-      <c r="A14" s="2" t="s">
-        <v>18</v>
+    <row r="16" spans="1:8">
+      <c r="A16" s="7" t="s">
+        <v>22</v>
       </c>
+      <c r="B16" s="6"/>
+      <c r="C16" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -24168,6 +24510,6 @@
     <hyperlink ref="A14" r:id="rId3" display="http://urbn.is/wealthcharts"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="77" orientation="portrait" r:id="rId4"/>
+  <pageSetup scale="77" orientation="landscape" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated text, final edits, ready for QC
</commit_message>
<xml_diff>
--- a/data/AssetSubsidies.xlsx
+++ b/data/AssetSubsidies.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\LHP\SMcKerna\Nine Charts 2017\Files for Ben\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bchartof/Projects/wealth-inequality-charts/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1020" windowWidth="17235" windowHeight="8760" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="1020" windowWidth="20600" windowHeight="16220" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Asset Subsidies--%s and dollars" sheetId="2" r:id="rId1"/>
@@ -24,12 +24,20 @@
     <definedName name="B">#REF!</definedName>
     <definedName name="C_">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="22">
   <si>
     <t>Expenditure</t>
   </si>
@@ -162,33 +170,56 @@
     <t>Size and Distribution of Select Asset-Building Tax Subsidies, 2017</t>
   </si>
   <si>
-    <t>FINAL CHART VALUES</t>
-  </si>
-  <si>
     <t>Dollars by taxpayer income quintile (billions)</t>
   </si>
   <si>
     <t>Total Expenditure and Share of Benefit, 2017</t>
   </si>
   <si>
-    <t>Comms: Use this sheet for downloadable data</t>
+    <t>Share by taxpayer income quintile (%)</t>
   </si>
   <si>
-    <t>Comms: Use this sheet for the data that will feed the graphic</t>
-  </si>
-  <si>
-    <t>Share by taxpayer income quintile</t>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Source:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Updated estimates from </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="10"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Steuerle et al. (2014).</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.0_);[Red]\(&quot;$&quot;#,##0.0\)"/>
   </numFmts>
-  <fonts count="9">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -248,7 +279,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,12 +288,6 @@
     </fill>
     <fill>
       <patternFill patternType="lightUp"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -275,10 +300,10 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -289,7 +314,7 @@
       <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
@@ -315,13 +340,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="13" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="13" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="14">
     <cellStyle name="Comma 2" xfId="1"/>
@@ -23816,9 +23843,9 @@
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -23846,31 +23873,14 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="Yu Gothic"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="DengXian"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -23898,23 +23908,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -24091,58 +24084,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="37" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" customWidth="1"/>
+    <col min="2" max="9" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="8"/>
+      <c r="I3" s="5"/>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="5" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -24161,11 +24155,11 @@
       <c r="F5">
         <v>72.599999999999994</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>63.6</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -24184,17 +24178,17 @@
       <c r="F6">
         <v>66.599999999999994</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>33.299999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="5" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G7" s="4"/>
+      <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -24213,11 +24207,11 @@
       <c r="F8">
         <v>62.8</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>194.447</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -24236,11 +24230,11 @@
       <c r="F9">
         <v>63</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>7.9720000000000013</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -24259,30 +24253,74 @@
       <c r="F10">
         <v>0.8</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>2.109</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="6"/>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A20" s="7"/>
+      <c r="B20" s="7"/>
+      <c r="C20" s="7"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A21" s="7"/>
+      <c r="B21" s="7"/>
+      <c r="C21" s="7"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A22" s="7"/>
+      <c r="B22" s="7"/>
+      <c r="C22" s="7"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7"/>
+      <c r="C24" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -24297,211 +24335,238 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="34.5703125" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" customWidth="1"/>
+    <col min="1" max="1" width="36" customWidth="1"/>
+    <col min="2" max="7" width="10.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B5" s="3">
         <v>6.3600000000000004E-2</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5" s="3">
         <v>0.69960000000000011</v>
       </c>
-      <c r="D5" s="4">
+      <c r="D5" s="3">
         <v>4.2612000000000005</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>12.402000000000001</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>46.1736</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>63.6</v>
       </c>
-      <c r="H5" s="4"/>
+      <c r="H5" s="3"/>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="4">
+      <c r="B6" s="3">
         <v>3.3299999999999996E-2</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6" s="3">
         <v>0.39959999999999996</v>
       </c>
-      <c r="D6" s="4">
+      <c r="D6" s="3">
         <v>2.7639</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>7.8920999999999992</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>22.177799999999994</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>33.266699999999993</v>
       </c>
-      <c r="H6" s="4"/>
+      <c r="H6" s="3"/>
     </row>
-    <row r="7" spans="1:8">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="4">
+      <c r="B8" s="3">
         <v>0.97223500000000007</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8" s="3">
         <v>7.1945390000000007</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <v>20.611381999999999</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>43.750575000000005</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>122.11271600000001</v>
       </c>
-      <c r="G8" s="4">
+      <c r="G8" s="3">
         <v>194.64144700000003</v>
       </c>
-      <c r="H8" s="4"/>
+      <c r="H8" s="3"/>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>12</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B9" s="3">
         <v>5.5804000000000006E-2</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9" s="3">
         <v>0.31090800000000007</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <v>0.97258400000000012</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>1.6023720000000004</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>5.0223600000000008</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>7.9640280000000017</v>
       </c>
-      <c r="H9" s="4"/>
+      <c r="H9" s="3"/>
     </row>
-    <row r="10" spans="1:8">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="4">
+      <c r="B10" s="3">
         <v>0.28260600000000002</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10" s="3">
         <v>0.8520359999999999</v>
       </c>
-      <c r="D10" s="4">
+      <c r="D10" s="3">
         <v>0.65589900000000001</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>0.30158700000000005</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>1.6872000000000002E-2</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>2.109</v>
       </c>
-      <c r="H10" s="4"/>
+      <c r="H10" s="3"/>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
-      <c r="A13" s="1" t="s">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" s="6" t="s">
         <v>16</v>
       </c>
+      <c r="B13" s="7"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7"/>
     </row>
-    <row r="14" spans="1:8">
-      <c r="A14" s="1" t="s">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="6" t="s">
         <v>14</v>
       </c>
+      <c r="B14" s="7"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="7"/>
     </row>
-    <row r="16" spans="1:8">
-      <c r="A16" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="7"/>
+      <c r="B15" s="7"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="7"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="8"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="7"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="7"/>
+      <c r="B17" s="7"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="7"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="7"/>
+      <c r="B18" s="7"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="7"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="7"/>
+      <c r="B19" s="7"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="7"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>